<commit_message>
Update description of methane pyrolysis dataset
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-pyrolysis.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-pyrolysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD20F31-9E7C-D249-A4C4-0B04B0D51951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF463D1-B247-3648-9071-9AC09BEA4812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33180" windowHeight="21260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lci" sheetId="1" r:id="rId1"/>
@@ -154,101 +154,101 @@
     <t>hydrogen production, gaseous, 100 bar, from methane pyrolysis</t>
   </si>
   <si>
-    <t>1 kg H2 produced by pyrolyzing methane. Pyrolysis processes decompose hydrocarbons into solid carbon and hydrogen at high temperatures (thermally or biologicalally). As no oxygen is present, no carbon oxides are formed, potentially eliminating the need for secondary processing steps such as the WGSR. The higher H2 concentration of the product gas stream also has considerable potential for minimising downstream clean-up processes. From a carbon-storage perspective, pyrolysis processes offer the advantage of storing a solid C-product as opposed to gaseous CO2. There is an allocation between the production of hydrogen and black carbon, based on their respective market value -- see Von Wald et al. 2020 for black carbon, and Florian Wirth, Green Hydrogen Production for Heavy-Duty Trucks, 2021, for hydrogen price in Switzerland. Source: Amjad Al-Qahtani, Brett Parkinson, Klaus Hellgardt, Nilay Shah, Gonzalo Guillen-Gosalbez, Uncovering the true cost of hydrogen production routes using life cycle monetisation, Applied Energy, 2021, https://doi.org/10.1016/j.apenergy.2020.115958.
+    <t>market value of hydrogen [CHF/kg]</t>
+  </si>
+  <si>
+    <t>market value of black carbon [CHF/kg]</t>
+  </si>
+  <si>
+    <t>allocation factor for hydrogen</t>
+  </si>
+  <si>
+    <t>hydrogen, gaseous, 100 bar</t>
+  </si>
+  <si>
+    <t>Infrastructure - membrane</t>
+  </si>
+  <si>
+    <t>market for palladium</t>
+  </si>
+  <si>
+    <t>palladium</t>
+  </si>
+  <si>
+    <t>market for steel, chromium steel 18/8</t>
+  </si>
+  <si>
+    <t>steel, chromium steel 18/8</t>
+  </si>
+  <si>
+    <t>Infrastructure - heat exchanger</t>
+  </si>
+  <si>
+    <t>market for tin</t>
+  </si>
+  <si>
+    <t>tin</t>
+  </si>
+  <si>
+    <t>Infrastructure - reactor</t>
+  </si>
+  <si>
+    <t>Infrastructure - filter</t>
+  </si>
+  <si>
+    <t>market for silicon carbide</t>
+  </si>
+  <si>
+    <t>silicon carbide</t>
+  </si>
+  <si>
+    <t>Infrastructure - burner</t>
+  </si>
+  <si>
+    <t>market for air compressor, screw-type compressor, 4kW</t>
+  </si>
+  <si>
+    <t>air compressor, screw-type compressor, 4kW</t>
+  </si>
+  <si>
+    <t>Infrastructure - compressor</t>
+  </si>
+  <si>
+    <t>market for natural gas, high pressure</t>
+  </si>
+  <si>
+    <t>natural gas, high pressure</t>
+  </si>
+  <si>
+    <t>market for tap water</t>
+  </si>
+  <si>
+    <t>tap water</t>
+  </si>
+  <si>
+    <t>RER</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>Assumed 90% of cooling water is released back.</t>
+  </si>
+  <si>
+    <t>Assumed 10% of cooling water is evaporated.</t>
+  </si>
+  <si>
+    <t>0.3 kWh/kWh H2 according to https://hydrogeneurope.eu/wp-content/uploads/2022/10/ewp_kompakt_pyrolyse_english_web.pdf</t>
+  </si>
+  <si>
+    <t>1.7 kWh CNG/kWh H2, according to https://hydrogeneurope.eu/wp-content/uploads/2022/10/ewp_kompakt_pyrolyse_english_web.pdf. 36 MJ/m3 CNG. Hence, 0.17 m3 CNG/kWh H2 and 5.67 m3 CNG/kg H2. Pastels et al. Show 6.57 m3.</t>
+  </si>
+  <si>
+    <t>1 kg H2 produced by pyrolyzing methane. NOTE: this is using a molten-metal reactor technology, particularly tin-intensive. Other technologies exist, which do not require metals to such an extent. Pyrolysis processes decompose hydrocarbons into solid carbon and hydrogen at high temperatures (thermally or biologicalally). As no oxygen is present, no carbon oxides are formed, potentially eliminating the need for secondary processing steps such as the WGSR. The higher H2 concentration of the product gas stream also has considerable potential for minimising downstream clean-up processes. From a carbon-storage perspective, pyrolysis processes offer the advantage of storing a solid C-product as opposed to gaseous CO2. There is an allocation between the production of hydrogen and black carbon, based on their respective market value -- see Von Wald et al. 2020 for black carbon, and Florian Wirth, Green Hydrogen Production for Heavy-Duty Trucks, 2021, for hydrogen price in Switzerland. Source: Amjad Al-Qahtani, Brett Parkinson, Klaus Hellgardt, Nilay Shah, Gonzalo Guillen-Gosalbez, Uncovering the true cost of hydrogen production routes using life cycle monetisation, Applied Energy, 2021, https://doi.org/10.1016/j.apenergy.2020.115958.
 The energy required is from DOI:10.1002/ceat.201600023. For pyrolysis, it can be provided both electrically and by burning some of the natural gas or pyrolysis products. For the comparison of technologies, electrical resistance heating is assumed, as use of this type of heating is deemed to be most practicable. The power requirement of 7.23 MWhel/ton H2 is based on thermodynamic calculations. These take into account both the energy losses during heat recovery and the compression power of 2 MWhel/ton H2, to compress pyrolysis hydrogen from 2 bar to 100 bar with three interim cooling stages. Inventories consolidated with numbers for infrastructures from Appendix A1 from Postels et al., 2016 https://doi.org/10.1016/j.ijhydene.2016.09.167. Missing input of quartz for reactor, as unavailable in ecoinvent.</t>
-  </si>
-  <si>
-    <t>market value of hydrogen [CHF/kg]</t>
-  </si>
-  <si>
-    <t>market value of black carbon [CHF/kg]</t>
-  </si>
-  <si>
-    <t>allocation factor for hydrogen</t>
-  </si>
-  <si>
-    <t>hydrogen, gaseous, 100 bar</t>
-  </si>
-  <si>
-    <t>Infrastructure - membrane</t>
-  </si>
-  <si>
-    <t>market for palladium</t>
-  </si>
-  <si>
-    <t>palladium</t>
-  </si>
-  <si>
-    <t>market for steel, chromium steel 18/8</t>
-  </si>
-  <si>
-    <t>steel, chromium steel 18/8</t>
-  </si>
-  <si>
-    <t>Infrastructure - heat exchanger</t>
-  </si>
-  <si>
-    <t>market for tin</t>
-  </si>
-  <si>
-    <t>tin</t>
-  </si>
-  <si>
-    <t>Infrastructure - reactor</t>
-  </si>
-  <si>
-    <t>Infrastructure - filter</t>
-  </si>
-  <si>
-    <t>market for silicon carbide</t>
-  </si>
-  <si>
-    <t>silicon carbide</t>
-  </si>
-  <si>
-    <t>Infrastructure - burner</t>
-  </si>
-  <si>
-    <t>market for air compressor, screw-type compressor, 4kW</t>
-  </si>
-  <si>
-    <t>air compressor, screw-type compressor, 4kW</t>
-  </si>
-  <si>
-    <t>Infrastructure - compressor</t>
-  </si>
-  <si>
-    <t>market for natural gas, high pressure</t>
-  </si>
-  <si>
-    <t>natural gas, high pressure</t>
-  </si>
-  <si>
-    <t>market for tap water</t>
-  </si>
-  <si>
-    <t>tap water</t>
-  </si>
-  <si>
-    <t>RER</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>Assumed 90% of cooling water is released back.</t>
-  </si>
-  <si>
-    <t>Assumed 10% of cooling water is evaporated.</t>
-  </si>
-  <si>
-    <t>0.3 kWh/kWh H2 according to https://hydrogeneurope.eu/wp-content/uploads/2022/10/ewp_kompakt_pyrolyse_english_web.pdf</t>
-  </si>
-  <si>
-    <t>1.7 kWh CNG/kWh H2, according to https://hydrogeneurope.eu/wp-content/uploads/2022/10/ewp_kompakt_pyrolyse_english_web.pdf. 36 MJ/m3 CNG. Hence, 0.17 m3 CNG/kWh H2 and 5.67 m3 CNG/kg H2. Pastels et al. Show 6.57 m3.</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
     <cellStyle name="Normal 11 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Per cent" xfId="5" builtinId="5"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T364"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -702,7 +702,7 @@
     <col min="5" max="5" width="26.5" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" style="5" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
@@ -769,7 +769,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
@@ -780,7 +780,7 @@
     </row>
     <row r="6" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="31">
         <v>12</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="7" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="31">
         <v>0.13</v>
@@ -808,7 +808,7 @@
     </row>
     <row r="8" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="32">
         <f>(1*B6)/((1*B6)+(3.91*B7))</f>
@@ -826,7 +826,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -840,7 +840,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -971,7 +971,7 @@
         <v>hydrogen, gaseous, 100 bar</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J14"/>
       <c r="K14" s="20"/>
@@ -986,9 +986,10 @@
     </row>
     <row r="15" spans="1:20" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="33">
+        <f>0.000011</f>
         <v>1.1E-5</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -1002,10 +1003,10 @@
         <v>12</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I15" s="12">
         <v>2</v>
@@ -1056,6 +1057,7 @@
         <v>35</v>
       </c>
       <c r="B16" s="33">
+        <f>0.00000733</f>
         <v>7.3300000000000001E-6</v>
       </c>
       <c r="C16" s="12" t="s">
@@ -1071,7 +1073,7 @@
         <v>36</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I16" s="12">
         <v>2</v>
@@ -1118,7 +1120,7 @@
     </row>
     <row r="17" spans="1:18" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="33">
         <v>2.5899999999999999E-3</v>
@@ -1133,10 +1135,10 @@
         <v>12</v>
       </c>
       <c r="G17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="I17" s="12">
         <v>2</v>
@@ -1173,7 +1175,7 @@
     </row>
     <row r="18" spans="1:18" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="33">
         <v>3.3599999999999998E-2</v>
@@ -1188,10 +1190,10 @@
         <v>12</v>
       </c>
       <c r="G18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="I18" s="12">
         <v>2</v>
@@ -1228,7 +1230,7 @@
     </row>
     <row r="19" spans="1:18" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="33">
         <v>5.0699999999999996E-4</v>
@@ -1243,10 +1245,10 @@
         <v>12</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I19" s="12">
         <v>2</v>
@@ -1283,7 +1285,7 @@
     </row>
     <row r="20" spans="1:18" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="33">
         <v>4.1999999999999996E-6</v>
@@ -1298,10 +1300,10 @@
         <v>12</v>
       </c>
       <c r="G20" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="I20" s="12">
         <v>2</v>
@@ -1338,7 +1340,7 @@
     </row>
     <row r="21" spans="1:18" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="33">
         <v>6.36E-8</v>
@@ -1353,10 +1355,10 @@
         <v>12</v>
       </c>
       <c r="G21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>59</v>
       </c>
       <c r="I21" s="12">
         <v>2</v>
@@ -1393,7 +1395,7 @@
     </row>
     <row r="22" spans="1:18" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="33">
         <v>5.67</v>
@@ -1408,10 +1410,10 @@
         <v>12</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I22" s="12">
         <v>2</v>
@@ -1448,7 +1450,7 @@
     </row>
     <row r="23" spans="1:18" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="33">
         <f>8.08*B8</f>
@@ -1464,7 +1466,7 @@
         <v>12</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I23" s="12">
         <v>2</v>
@@ -1501,7 +1503,7 @@
     </row>
     <row r="24" spans="1:18" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="33">
         <f>B23*0.9/1000</f>
@@ -1511,13 +1513,13 @@
         <v>17</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>14</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I24" s="12">
         <v>0</v>
@@ -1534,7 +1536,7 @@
     </row>
     <row r="25" spans="1:18" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="33">
         <f>B23*0.1/1000</f>
@@ -1550,7 +1552,7 @@
         <v>14</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J25"/>
       <c r="K25" s="20"/>
@@ -1583,7 +1585,7 @@
         <v>20</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I26" s="12">
         <v>2</v>

</xml_diff>